<commit_message>
Amélioration du placement des points
</commit_message>
<xml_diff>
--- a/_data/data.xlsx
+++ b/_data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\briac\git\bab-a-velo\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10786990-2A6B-4582-BACE-07411BE9AE55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6588D3A-31CE-4B92-B723-8682D7EE59B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5BF2F094-2AF3-4F97-9DFC-FB300D796DC2}"/>
+    <workbookView xWindow="-1248" yWindow="1896" windowWidth="22236" windowHeight="9816" activeTab="1" xr2:uid="{5BF2F094-2AF3-4F97-9DFC-FB300D796DC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Trajets" sheetId="1" r:id="rId1"/>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF6C08D-8714-4B59-AF4B-AB3081A3DF97}">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="H82" sqref="H82"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H91" sqref="H2:H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,14 +955,14 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
         <v>72</v>
       </c>
       <c r="H16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>{ start: "Boucau", end: "LaBarre", difficulty: 0, time: 17, className:"bateau" },</v>
+        <v>{ start: "Boucau", end: "LaBarre", difficulty: 0, time: 12, className:"bateau" },</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -2340,9 +2340,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G101">
-    <sortCondition ref="B2:B101" customList="Mora,Tarnos,Humere,Forges,Matignon,LaBarre,Boucau,Blancpignon,Seque,Habas,ChambreAmour,Forum,5Cantons,PlaceGascons,Arrousets,Bayonne,SaintCharles,SaintFrederic,Mousserolles,EuroFret,Biarritz,Anglet,Marracq,Aeroport,Mendixta,Technocite,Iraty,Milady,Bassussary,Izarbel,LoreLanda,Ilbarritz,Arcangues,Arbonne,Uhabia,Bidart"/>
-    <sortCondition ref="C2:C101" customList="Mora,Tarnos,Humere,Forges,Matignon,LaBarre,Boucau,Blancpignon,Seque,Habas,ChambreAmour,Forum,5Cantons,PlaceGascons,Arrousets,Bayonne,SaintCharles,SaintFrederic,Mousserolles,EuroFret,Biarritz,Anglet,Marracq,Aeroport,Mendixta,Technocite,Iraty,Milady,Bassussary,Izarbel,LoreLanda,Ilbarritz,Arcangues,Arbonne,Uhabia,Bidart"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G91">
+    <sortCondition ref="B2:B91" customList="Mora,Tarnos,Humere,Forges,Matignon,LaBarre,Boucau,Blancpignon,Seque,Habas,ChambreAmour,Forum,5Cantons,PlaceGascons,Arrousets,Bayonne,SaintCharles,SaintFrederic,Mousserolles,EuroFret,Biarritz,Anglet,Marracq,Aeroport,Mendixta,Technocite,Iraty,Milady,Bassussary,Izarbel,LoreLanda,Ilbarritz,Arcangues,Arbonne,Uhabia,Bidart"/>
+    <sortCondition ref="C2:C91" customList="Mora,Tarnos,Humere,Forges,Matignon,LaBarre,Boucau,Blancpignon,Seque,Habas,ChambreAmour,Forum,5Cantons,PlaceGascons,Arrousets,Bayonne,SaintCharles,SaintFrederic,Mousserolles,EuroFret,Biarritz,Anglet,Marracq,Aeroport,Mendixta,Technocite,Iraty,Milady,Bassussary,Izarbel,LoreLanda,Ilbarritz,Arcangues,Arbonne,Uhabia,Bidart"/>
   </sortState>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C101:C242 B101:B165 B2:C101" xr:uid="{3B456A81-72D1-4F29-81DE-3CBEA4D6D3A6}">
@@ -2357,8 +2357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5480694-7368-450D-8AFA-446FD6A20927}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2604,38 +2604,38 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C14">
-        <v>318</v>
+        <v>526</v>
       </c>
       <c r="D14">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="F14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>"5cantons": {label:"Cinq Cantons - Chassin", x:318, y:257},</v>
+        <v>"PlaceGascons": {label:"Place des Gascons", x:526, y:262},</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C15">
-        <v>526</v>
+        <v>313</v>
       </c>
       <c r="D15">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="F15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>"PlaceGascons": {label:"Place des Gascons", x:526, y:262},</v>
+        <v>"5cantons": {label:"Cinq Cantons - Chassin", x:313, y:269},</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2700,14 +2700,14 @@
         <v>43</v>
       </c>
       <c r="C19">
-        <v>554</v>
+        <v>564</v>
       </c>
       <c r="D19">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="F19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>"SaintFrederic": {label:"Zone Saint Frédéric", x:554, y:327},</v>
+        <v>"SaintFrederic": {label:"Zone Saint Frédéric", x:564, y:317},</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2910,38 +2910,38 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C31">
-        <v>212</v>
+        <v>269</v>
       </c>
       <c r="D31">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>"Izarbel": {label:"Technopôle Izarbel", x:212, y:535},</v>
+        <v>"LoreLanda": {label:"Pôle Lore Landa", x:269, y:534},</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32">
-        <v>269</v>
+        <v>218</v>
       </c>
       <c r="D32">
-        <v>534</v>
+        <v>545</v>
       </c>
       <c r="F32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>"LoreLanda": {label:"Pôle Lore Landa", x:269, y:534},</v>
+        <v>"Izarbel": {label:"Technopôle Izarbel", x:218, y:545},</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -3038,8 +3038,8 @@
       <c r="F57" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D58">
-    <sortCondition ref="D2:D58"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D57">
+    <sortCondition ref="D2:D57"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>